<commit_message>
Parties 1 et 2.
</commit_message>
<xml_diff>
--- a/Saison24/DonnéesCSV/Saisie des points.xlsx
+++ b/Saison24/DonnéesCSV/Saisie des points.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="151">
   <si>
     <t xml:space="preserve">Saisi des points</t>
   </si>
@@ -328,6 +328,12 @@
     <t xml:space="preserve">Caroline</t>
   </si>
   <si>
+    <t xml:space="preserve">Coulombe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sylvain</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lapierre</t>
   </si>
   <si>
@@ -340,9 +346,6 @@
     <t xml:space="preserve">Perron</t>
   </si>
   <si>
-    <t xml:space="preserve">Sylvain</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sirois</t>
   </si>
   <si>
@@ -454,6 +457,18 @@
     <t xml:space="preserve">Félix</t>
   </si>
   <si>
+    <t xml:space="preserve">Louis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lemyre (Faciles)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LeBlanc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Élizabeth</t>
+  </si>
+  <si>
     <t xml:space="preserve">Turpin</t>
   </si>
   <si>
@@ -464,18 +479,6 @@
   </si>
   <si>
     <t xml:space="preserve">James</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lemyre (Faciles)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LeBlanc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Élizabeth</t>
   </si>
 </sst>
 </file>
@@ -731,7 +734,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblJoueurs" displayName="tblJoueurs" ref="A1:K82" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblÉquipes" displayName="tblÉquipes" ref="A1:E8" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E8"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="NoÉquipe"/>
+    <tableColumn id="2" name="NomÉquipe"/>
+    <tableColumn id="3" name="PosFinale"/>
+    <tableColumn id="4" name="Carillon"/>
+    <tableColumn id="5" name="NoÉquipe2"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblJoueurs" displayName="tblJoueurs" ref="A1:K82" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:K82"/>
   <tableColumns count="11">
     <tableColumn id="1" name="NoÉquipe"/>
@@ -745,19 +761,6 @@
     <tableColumn id="9" name="NoÉquipe2"/>
     <tableColumn id="10" name="NoJoueur2"/>
     <tableColumn id="11" name="Nom complet"/>
-  </tableColumns>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblÉquipes" displayName="tblÉquipes" ref="A1:E8" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E8"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="NoÉquipe"/>
-    <tableColumn id="2" name="NomÉquipe"/>
-    <tableColumn id="3" name="PosFinale"/>
-    <tableColumn id="4" name="Carillon"/>
-    <tableColumn id="5" name="NoÉquipe2"/>
   </tableColumns>
 </table>
 </file>
@@ -879,7 +882,7 @@
       <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.57"/>
@@ -1198,18 +1201,18 @@
       <c r="F13" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="G13" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>99</v>
+      <c r="G13" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H13" s="1" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="K13" s="1" t="str">
+      <c r="K13" s="1" t="e">
         <f aca="false">F13&amp;","&amp;G13&amp;","&amp;H13&amp;","&amp;I13</f>
-        <v>22,7,99,40</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1404,10 +1407,10 @@
         <v>7</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C22" s="1" t="str">
-        <v>Danielle Turpin</v>
+        <v>Absent Absent</v>
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="1" t="n">
@@ -1432,10 +1435,10 @@
         <v>7</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C23" s="1" t="str">
-        <v>James Falconer</v>
+        <v>Catherine NA</v>
       </c>
       <c r="D23" s="5"/>
       <c r="F23" s="1" t="n">
@@ -1460,10 +1463,10 @@
         <v>7</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1" t="str">
-        <v>Absent Absent</v>
+        <v>Louis NA</v>
       </c>
       <c r="D24" s="5"/>
       <c r="F24" s="1" t="n">
@@ -1488,10 +1491,10 @@
         <v>7</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1" t="str">
-        <v>Catherine NA</v>
+        <v>Étienne Lemyre (Faciles)</v>
       </c>
       <c r="D25" s="5"/>
       <c r="F25" s="1" t="n">
@@ -1516,10 +1519,10 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1" t="str">
-        <v>Louis NA</v>
+        <v>Élizabeth LeBlanc</v>
       </c>
       <c r="D26" s="5"/>
       <c r="F26" s="1" t="n">
@@ -1544,10 +1547,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="C27" s="1" t="str">
-        <v>Étienne Lemyre (Faciles)</v>
+        <v>NA Les Faciles à cuire</v>
       </c>
       <c r="D27" s="5"/>
       <c r="F27" s="1" t="n">
@@ -1568,14 +1571,14 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B28" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="C28" s="1" t="str">
-        <v>Élizabeth LeBlanc</v>
+      <c r="A28" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B28" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C28" s="1" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D28" s="5"/>
       <c r="F28" s="1" t="n">
@@ -1596,14 +1599,14 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B29" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="C29" s="1" t="str">
-        <v>NA Les Faciles à cuire</v>
+      <c r="A29" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B29" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C29" s="1" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>40</v>
@@ -1684,7 +1687,7 @@
       </c>
       <c r="H32" s="1" t="n">
         <f aca="false">B22</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I32" s="1" t="n">
         <f aca="false">D22</f>
@@ -1703,7 +1706,7 @@
       </c>
       <c r="H33" s="1" t="n">
         <f aca="false">B23</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I33" s="1" t="n">
         <f aca="false">D23</f>
@@ -1721,7 +1724,7 @@
       </c>
       <c r="H34" s="1" t="n">
         <f aca="false">B24</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I34" s="1" t="n">
         <f aca="false">D24</f>
@@ -1739,7 +1742,7 @@
       </c>
       <c r="H35" s="1" t="n">
         <f aca="false">B25</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I35" s="1" t="n">
         <f aca="false">D25</f>
@@ -1757,7 +1760,7 @@
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">B26</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I36" s="1" t="n">
         <f aca="false">D26</f>
@@ -1775,7 +1778,7 @@
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">B27</f>
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="I37" s="1" t="n">
         <f aca="false">D27</f>
@@ -1787,13 +1790,13 @@
         <f aca="false">$B$2</f>
         <v>22</v>
       </c>
-      <c r="G38" s="1" t="n">
+      <c r="G38" s="1" t="e">
         <f aca="false">A28</f>
-        <v>7</v>
-      </c>
-      <c r="H38" s="1" t="n">
+        <v>#N/A</v>
+      </c>
+      <c r="H38" s="1" t="e">
         <f aca="false">B28</f>
-        <v>12</v>
+        <v>#N/A</v>
       </c>
       <c r="I38" s="1" t="n">
         <f aca="false">D28</f>
@@ -1805,13 +1808,13 @@
         <f aca="false">$B$2</f>
         <v>22</v>
       </c>
-      <c r="G39" s="1" t="n">
+      <c r="G39" s="1" t="e">
         <f aca="false">A29</f>
-        <v>7</v>
-      </c>
-      <c r="H39" s="1" t="n">
+        <v>#N/A</v>
+      </c>
+      <c r="H39" s="1" t="e">
         <f aca="false">B29</f>
-        <v>99</v>
+        <v>#N/A</v>
       </c>
       <c r="I39" s="1" t="n">
         <f aca="false">D29</f>
@@ -1958,7 +1961,7 @@
       <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.14"/>
@@ -2132,10 +2135,10 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.85"/>
@@ -2188,28 +2191,28 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="0" t="n">
+      <c r="G2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I2" s="1" t="n">
@@ -2229,28 +2232,28 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="0" t="n">
+      <c r="G3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I3" s="1" t="n">
@@ -2267,28 +2270,28 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="G4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
@@ -2305,28 +2308,28 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="A5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="0" t="n">
+      <c r="G5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I5" s="1" t="n">
@@ -2343,28 +2346,28 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="0" t="n">
+      <c r="G6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="n">
@@ -2381,28 +2384,28 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="0" t="n">
+      <c r="G7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="n">
@@ -2432,28 +2435,28 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="A8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="0" t="n">
+      <c r="G8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="n">
@@ -2482,28 +2485,28 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" s="0" t="n">
+      <c r="A9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="0" t="n">
+      <c r="G9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="n">
@@ -2532,28 +2535,28 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="0" t="n">
+      <c r="A10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="0" t="n">
+      <c r="G10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="1" t="n">
@@ -2582,28 +2585,28 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="0" t="n">
+      <c r="A11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="0" t="n">
+      <c r="G11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="n">
@@ -2632,28 +2635,28 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" s="0" t="n">
+      <c r="A12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="0" t="n">
+      <c r="G12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I12" s="1" t="n">
@@ -2682,28 +2685,28 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="A13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="0" t="n">
+      <c r="G13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I13" s="1" t="n">
@@ -2732,28 +2735,28 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="A14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="0" t="n">
+      <c r="G14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="n">
@@ -2782,28 +2785,28 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="A15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" s="0" t="n">
+      <c r="G15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I15" s="1" t="n">
@@ -2820,28 +2823,28 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="A16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="0" t="n">
+      <c r="G16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
@@ -2858,28 +2861,28 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B17" s="0" t="n">
+      <c r="A17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="0" t="n">
+      <c r="G17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I17" s="1" t="n">
@@ -2896,28 +2899,28 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B18" s="0" t="n">
+      <c r="A18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" s="0" t="n">
+      <c r="G18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="n">
@@ -2944,28 +2947,28 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C19" s="0" t="s">
+      <c r="A19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H19" s="0" t="n">
+      <c r="G19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="n">
@@ -2991,28 +2994,28 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B20" s="0" t="n">
+      <c r="A20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="0" t="n">
+      <c r="G20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="n">
@@ -3038,28 +3041,28 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B21" s="0" t="n">
+      <c r="A21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" s="0" t="n">
+      <c r="G21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="n">
@@ -3085,28 +3088,28 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B22" s="0" t="n">
+      <c r="A22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H22" s="0" t="n">
+      <c r="G22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="n">
@@ -3132,28 +3135,28 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B23" s="0" t="n">
+      <c r="A23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H23" s="0" t="n">
+      <c r="G23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I23" s="1" t="n">
@@ -3179,28 +3182,28 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" s="0" t="s">
+      <c r="A24" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" s="0" t="n">
+      <c r="G24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I24" s="1" t="n">
@@ -3226,28 +3229,28 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C25" s="0" t="s">
+      <c r="A25" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H25" s="0" t="n">
+      <c r="G25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I25" s="1" t="n">
@@ -3273,28 +3276,28 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C26" s="0" t="s">
+      <c r="A26" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H26" s="0" t="n">
+      <c r="G26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I26" s="1" t="n">
@@ -3320,28 +3323,28 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C27" s="0" t="s">
+      <c r="A27" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H27" s="0" t="n">
+      <c r="G27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I27" s="1" t="n">
@@ -3358,28 +3361,28 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B28" s="0" t="n">
+      <c r="A28" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H28" s="0" t="n">
+      <c r="G28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I28" s="1" t="n">
@@ -3396,28 +3399,28 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B29" s="0" t="n">
+      <c r="A29" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B29" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H29" s="0" t="n">
+      <c r="G29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I29" s="1" t="n">
@@ -3434,28 +3437,28 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C30" s="0" t="s">
+      <c r="A30" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H30" s="0" t="n">
+      <c r="G30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I30" s="1" t="n">
@@ -3472,28 +3475,28 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B31" s="0" t="n">
+      <c r="A31" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B31" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H31" s="0" t="n">
+      <c r="G31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I31" s="1" t="n">
@@ -3510,28 +3513,28 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B32" s="0" t="n">
+      <c r="A32" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H32" s="0" t="n">
+      <c r="G32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I32" s="1" t="n">
@@ -3548,28 +3551,28 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="0" t="s">
+      <c r="A33" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F33" s="0" t="s">
+      <c r="F33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H33" s="0" t="n">
+      <c r="G33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I33" s="1" t="n">
@@ -3586,28 +3589,28 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C34" s="0" t="s">
+      <c r="A34" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="F34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H34" s="0" t="n">
+      <c r="G34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I34" s="1" t="n">
@@ -3624,28 +3627,28 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C35" s="0" t="s">
+      <c r="A35" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="F35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H35" s="0" t="n">
+      <c r="G35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I35" s="1" t="n">
@@ -3662,28 +3665,28 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C36" s="0" t="s">
+      <c r="A36" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="F36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H36" s="0" t="n">
+      <c r="G36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I36" s="1" t="n">
@@ -3700,28 +3703,28 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B37" s="0" t="n">
+      <c r="A37" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="F37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H37" s="0" t="n">
+      <c r="G37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I37" s="1" t="n">
@@ -3738,28 +3741,28 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B38" s="0" t="n">
+      <c r="A38" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H38" s="0" t="n">
+      <c r="G38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I38" s="1" t="n">
@@ -3776,28 +3779,28 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C39" s="0" t="s">
+      <c r="A39" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="F39" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H39" s="0" t="n">
+      <c r="G39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I39" s="1" t="n">
@@ -3814,28 +3817,28 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B40" s="0" t="n">
+      <c r="A40" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B40" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="F40" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H40" s="0" t="n">
+      <c r="G40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H40" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I40" s="1" t="n">
@@ -3852,28 +3855,28 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B41" s="0" t="n">
+      <c r="A41" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B41" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F41" s="0" t="s">
+      <c r="F41" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H41" s="0" t="n">
+      <c r="G41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I41" s="1" t="n">
@@ -3890,28 +3893,28 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>99</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H42" s="0" t="n">
+      <c r="A42" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I42" s="1" t="n">
@@ -3920,75 +3923,75 @@
       </c>
       <c r="J42" s="1" t="n">
         <f aca="false">tblJoueurs!$B42</f>
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="K42" s="1" t="str">
         <f aca="false">tblJoueurs!$D42 &amp; " " &amp;tblJoueurs!$C42</f>
-        <v>NA Les Herbizarres</v>
+        <v>Sylvain Coulombe</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G43" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H43" s="0" t="n">
-        <v>4</v>
+      <c r="A43" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="I43" s="1" t="n">
         <f aca="false">tblJoueurs!$A43</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J43" s="1" t="n">
         <f aca="false">tblJoueurs!$B43</f>
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="K43" s="1" t="str">
         <f aca="false">tblJoueurs!$D43 &amp; " " &amp;tblJoueurs!$C43</f>
-        <v>Bruno Lapierre</v>
+        <v>NA Les Herbizarres</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="A44" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B44" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C44" s="0" t="s">
+      <c r="B44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H44" s="0" t="n">
-        <v>1</v>
+      <c r="D44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I44" s="1" t="n">
         <f aca="false">tblJoueurs!$A44</f>
@@ -3996,37 +3999,37 @@
       </c>
       <c r="J44" s="1" t="n">
         <f aca="false">tblJoueurs!$B44</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K44" s="1" t="str">
         <f aca="false">tblJoueurs!$D44 &amp; " " &amp;tblJoueurs!$C44</f>
-        <v>Julie Bernier</v>
+        <v>Bruno Lapierre</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B45" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D45" s="0" t="s">
+      <c r="B45" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E45" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="F45" s="0" t="s">
+      <c r="D45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H45" s="0" t="n">
-        <v>2</v>
+      <c r="G45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I45" s="1" t="n">
         <f aca="false">tblJoueurs!$A45</f>
@@ -4034,37 +4037,37 @@
       </c>
       <c r="J45" s="1" t="n">
         <f aca="false">tblJoueurs!$B45</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K45" s="1" t="str">
         <f aca="false">tblJoueurs!$D45 &amp; " " &amp;tblJoueurs!$C45</f>
-        <v>Sylvain Perron</v>
+        <v>Julie Bernier</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+      <c r="A46" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B46" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C46" s="0" t="s">
+      <c r="B46" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="F46" s="0" t="s">
+      <c r="D46" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H46" s="0" t="n">
-        <v>0</v>
+      <c r="G46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="I46" s="1" t="n">
         <f aca="false">tblJoueurs!$A46</f>
@@ -4072,37 +4075,37 @@
       </c>
       <c r="J46" s="1" t="n">
         <f aca="false">tblJoueurs!$B46</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K46" s="1" t="str">
         <f aca="false">tblJoueurs!$D46 &amp; " " &amp;tblJoueurs!$C46</f>
-        <v>Martin Sirois</v>
+        <v>Sylvain Perron</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B47" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C47" s="0" t="s">
+      <c r="B47" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="F47" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H47" s="0" t="n">
-        <v>3</v>
+      <c r="E47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="I47" s="1" t="n">
         <f aca="false">tblJoueurs!$A47</f>
@@ -4110,37 +4113,37 @@
       </c>
       <c r="J47" s="1" t="n">
         <f aca="false">tblJoueurs!$B47</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K47" s="1" t="str">
         <f aca="false">tblJoueurs!$D47 &amp; " " &amp;tblJoueurs!$C47</f>
-        <v>Didier Garriguet</v>
+        <v>Martin Sirois</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
+      <c r="A48" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B48" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C48" s="0" t="s">
+      <c r="B48" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="F48" s="0" t="s">
+      <c r="E48" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H48" s="0" t="n">
-        <v>0</v>
+      <c r="G48" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I48" s="1" t="n">
         <f aca="false">tblJoueurs!$A48</f>
@@ -4148,36 +4151,36 @@
       </c>
       <c r="J48" s="1" t="n">
         <f aca="false">tblJoueurs!$B48</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K48" s="1" t="str">
         <f aca="false">tblJoueurs!$D48 &amp; " " &amp;tblJoueurs!$C48</f>
-        <v>Jean-Sébastien Provencal</v>
+        <v>Didier Garriguet</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
+      <c r="A49" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B49" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" s="0" t="s">
+      <c r="B49" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G49" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H49" s="0" t="n">
+      <c r="G49" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I49" s="1" t="n">
@@ -4186,37 +4189,37 @@
       </c>
       <c r="J49" s="1" t="n">
         <f aca="false">tblJoueurs!$B49</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K49" s="1" t="str">
         <f aca="false">tblJoueurs!$D49 &amp; " " &amp;tblJoueurs!$C49</f>
-        <v>Absent Absent</v>
+        <v>Jean-Sébastien Provencal</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
+      <c r="A50" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B50" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="F50" s="0" t="s">
+      <c r="B50" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G50" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H50" s="0" t="n">
-        <v>3</v>
+      <c r="G50" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="I50" s="1" t="n">
         <f aca="false">tblJoueurs!$A50</f>
@@ -4224,36 +4227,36 @@
       </c>
       <c r="J50" s="1" t="n">
         <f aca="false">tblJoueurs!$B50</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K50" s="1" t="str">
         <f aca="false">tblJoueurs!$D50 &amp; " " &amp;tblJoueurs!$C50</f>
-        <v>Marlène Savard</v>
+        <v>Absent Absent</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B51" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="C51" s="0" t="s">
+      <c r="B51" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D51" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F51" s="0" t="s">
+      <c r="E51" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H51" s="0" t="n">
+      <c r="G51" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I51" s="1" t="n">
@@ -4262,37 +4265,37 @@
       </c>
       <c r="J51" s="1" t="n">
         <f aca="false">tblJoueurs!$B51</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K51" s="1" t="str">
         <f aca="false">tblJoueurs!$D51 &amp; " " &amp;tblJoueurs!$C51</f>
-        <v>François Lavoie</v>
+        <v>Marlène Savard</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
+      <c r="A52" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B52" s="0" t="n">
-        <v>99</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G52" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H52" s="0" t="n">
-        <v>0</v>
+      <c r="B52" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I52" s="1" t="n">
         <f aca="false">tblJoueurs!$A52</f>
@@ -4300,75 +4303,75 @@
       </c>
       <c r="J52" s="1" t="n">
         <f aca="false">tblJoueurs!$B52</f>
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="K52" s="1" t="str">
         <f aca="false">tblJoueurs!$D52 &amp; " " &amp;tblJoueurs!$C52</f>
-        <v>NA Les Méthos précieux</v>
+        <v>François Lavoie</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F53" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H53" s="0" t="n">
-        <v>1</v>
+      <c r="A53" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B53" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G53" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="I53" s="1" t="n">
         <f aca="false">tblJoueurs!$A53</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J53" s="1" t="n">
         <f aca="false">tblJoueurs!$B53</f>
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="K53" s="1" t="str">
         <f aca="false">tblJoueurs!$D53 &amp; " " &amp;tblJoueurs!$C53</f>
-        <v>Stéphane Mongeau</v>
+        <v>NA Les Méthos précieux</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
+      <c r="A54" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B54" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C54" s="0" t="s">
+      <c r="B54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D54" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G54" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H54" s="0" t="n">
-        <v>3</v>
+      <c r="D54" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I54" s="1" t="n">
         <f aca="false">tblJoueurs!$A54</f>
@@ -4376,37 +4379,37 @@
       </c>
       <c r="J54" s="1" t="n">
         <f aca="false">tblJoueurs!$B54</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K54" s="1" t="str">
         <f aca="false">tblJoueurs!$D54 &amp; " " &amp;tblJoueurs!$C54</f>
-        <v>Pierre-Olivier Julien</v>
+        <v>Stéphane Mongeau</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+      <c r="A55" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B55" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C55" s="0" t="s">
+      <c r="B55" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F55" s="0" t="s">
+      <c r="E55" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G55" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H55" s="0" t="n">
-        <v>2</v>
+      <c r="G55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I55" s="1" t="n">
         <f aca="false">tblJoueurs!$A55</f>
@@ -4414,37 +4417,37 @@
       </c>
       <c r="J55" s="1" t="n">
         <f aca="false">tblJoueurs!$B55</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K55" s="1" t="str">
         <f aca="false">tblJoueurs!$D55 &amp; " " &amp;tblJoueurs!$C55</f>
-        <v>Julien Bérard-Chagnon</v>
+        <v>Pierre-Olivier Julien</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
+      <c r="A56" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B56" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C56" s="0" t="s">
+      <c r="B56" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D56" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="F56" s="0" t="s">
+      <c r="D56" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G56" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H56" s="0" t="n">
-        <v>0</v>
+      <c r="G56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="I56" s="1" t="n">
         <f aca="false">tblJoueurs!$A56</f>
@@ -4452,37 +4455,37 @@
       </c>
       <c r="J56" s="1" t="n">
         <f aca="false">tblJoueurs!$B56</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K56" s="1" t="str">
         <f aca="false">tblJoueurs!$D56 &amp; " " &amp;tblJoueurs!$C56</f>
-        <v>Patrick Charbonneau</v>
+        <v>Julien Bérard-Chagnon</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
+      <c r="A57" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B57" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C57" s="0" t="s">
+      <c r="B57" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D57" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="F57" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G57" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H57" s="0" t="n">
-        <v>4</v>
+      <c r="E57" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G57" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="I57" s="1" t="n">
         <f aca="false">tblJoueurs!$A57</f>
@@ -4490,37 +4493,37 @@
       </c>
       <c r="J57" s="1" t="n">
         <f aca="false">tblJoueurs!$B57</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K57" s="1" t="str">
         <f aca="false">tblJoueurs!$D57 &amp; " " &amp;tblJoueurs!$C57</f>
-        <v>Keven Bosa</v>
+        <v>Patrick Charbonneau</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
+      <c r="A58" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B58" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C58" s="0" t="s">
+      <c r="B58" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="F58" s="0" t="s">
+      <c r="E58" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G58" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H58" s="0" t="n">
-        <v>0</v>
+      <c r="G58" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I58" s="1" t="n">
         <f aca="false">tblJoueurs!$A58</f>
@@ -4528,36 +4531,36 @@
       </c>
       <c r="J58" s="1" t="n">
         <f aca="false">tblJoueurs!$B58</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K58" s="1" t="str">
         <f aca="false">tblJoueurs!$D58 &amp; " " &amp;tblJoueurs!$C58</f>
-        <v>Étienne Rassart</v>
+        <v>Keven Bosa</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
+      <c r="A59" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B59" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C59" s="0" t="s">
+      <c r="B59" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D59" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="F59" s="0" t="s">
+      <c r="E59" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G59" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H59" s="0" t="n">
+      <c r="G59" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I59" s="1" t="n">
@@ -4566,36 +4569,36 @@
       </c>
       <c r="J59" s="1" t="n">
         <f aca="false">tblJoueurs!$B59</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K59" s="1" t="str">
         <f aca="false">tblJoueurs!$D59 &amp; " " &amp;tblJoueurs!$C59</f>
-        <v>Daphné Allard Gervais</v>
+        <v>Étienne Rassart</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
+      <c r="A60" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B60" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C60" s="0" t="s">
+      <c r="B60" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D60" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F60" s="0" t="s">
+      <c r="E60" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G60" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H60" s="0" t="n">
+      <c r="G60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I60" s="1" t="n">
@@ -4604,36 +4607,36 @@
       </c>
       <c r="J60" s="1" t="n">
         <f aca="false">tblJoueurs!$B60</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K60" s="1" t="str">
         <f aca="false">tblJoueurs!$D60 &amp; " " &amp;tblJoueurs!$C60</f>
-        <v>Emy Bourdages</v>
+        <v>Daphné Allard Gervais</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
+      <c r="A61" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B61" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="C61" s="0" t="s">
+      <c r="B61" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D61" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="F61" s="0" t="s">
+      <c r="E61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G61" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H61" s="0" t="n">
+      <c r="G61" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I61" s="1" t="n">
@@ -4642,36 +4645,36 @@
       </c>
       <c r="J61" s="1" t="n">
         <f aca="false">tblJoueurs!$B61</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K61" s="1" t="str">
         <f aca="false">tblJoueurs!$D61 &amp; " " &amp;tblJoueurs!$C61</f>
-        <v>David Binet</v>
+        <v>Emy Bourdages</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
+      <c r="A62" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B62" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="F62" s="0" t="s">
+      <c r="B62" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G62" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H62" s="0" t="n">
+      <c r="G62" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I62" s="1" t="n">
@@ -4680,36 +4683,36 @@
       </c>
       <c r="J62" s="1" t="n">
         <f aca="false">tblJoueurs!$B62</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K62" s="1" t="str">
         <f aca="false">tblJoueurs!$D62 &amp; " " &amp;tblJoueurs!$C62</f>
-        <v>Absent Absent</v>
+        <v>David Binet</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+      <c r="A63" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B63" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F63" s="0" t="s">
+      <c r="B63" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G63" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H63" s="0" t="n">
+      <c r="G63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I63" s="1" t="n">
@@ -4718,36 +4721,36 @@
       </c>
       <c r="J63" s="1" t="n">
         <f aca="false">tblJoueurs!$B63</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K63" s="1" t="str">
         <f aca="false">tblJoueurs!$D63 &amp; " " &amp;tblJoueurs!$C63</f>
-        <v>François Sergerie</v>
+        <v>Absent Absent</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
+      <c r="A64" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B64" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="C64" s="0" t="s">
+      <c r="B64" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D64" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="F64" s="0" t="s">
+      <c r="D64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G64" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H64" s="0" t="n">
+      <c r="G64" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I64" s="1" t="n">
@@ -4756,36 +4759,36 @@
       </c>
       <c r="J64" s="1" t="n">
         <f aca="false">tblJoueurs!$B64</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K64" s="1" t="str">
         <f aca="false">tblJoueurs!$D64 &amp; " " &amp;tblJoueurs!$C64</f>
-        <v>Arnaud Bouchard-Santerre</v>
+        <v>François Sergerie</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+      <c r="A65" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B65" s="0" t="n">
-        <v>99</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F65" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G65" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H65" s="0" t="n">
+      <c r="B65" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G65" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H65" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I65" s="1" t="n">
@@ -4794,75 +4797,75 @@
       </c>
       <c r="J65" s="1" t="n">
         <f aca="false">tblJoueurs!$B65</f>
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="K65" s="1" t="str">
         <f aca="false">tblJoueurs!$D65 &amp; " " &amp;tblJoueurs!$C65</f>
-        <v>NA Les 12e meilleurs</v>
+        <v>Arnaud Bouchard-Santerre</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B66" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G66" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H66" s="0" t="n">
+      <c r="A66" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B66" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H66" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I66" s="1" t="n">
         <f aca="false">tblJoueurs!$A66</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J66" s="1" t="n">
         <f aca="false">tblJoueurs!$B66</f>
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="K66" s="1" t="str">
         <f aca="false">tblJoueurs!$D66 &amp; " " &amp;tblJoueurs!$C66</f>
-        <v>Philippe Bérubé</v>
+        <v>NA Les 12e meilleurs</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B67" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C67" s="0" t="s">
+      <c r="A67" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B67" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D67" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="F67" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G67" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H67" s="0" t="n">
-        <v>4</v>
+      <c r="E67" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G67" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H67" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="I67" s="1" t="n">
         <f aca="false">tblJoueurs!$A67</f>
@@ -4870,37 +4873,37 @@
       </c>
       <c r="J67" s="1" t="n">
         <f aca="false">tblJoueurs!$B67</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K67" s="1" t="str">
         <f aca="false">tblJoueurs!$D67 &amp; " " &amp;tblJoueurs!$C67</f>
-        <v>Tony Labillois</v>
+        <v>Philippe Bérubé</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B68" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C68" s="0" t="s">
+      <c r="A68" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B68" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D68" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="F68" s="0" t="s">
+      <c r="E68" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G68" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H68" s="0" t="n">
-        <v>2</v>
+      <c r="G68" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H68" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I68" s="1" t="n">
         <f aca="false">tblJoueurs!$A68</f>
@@ -4908,37 +4911,37 @@
       </c>
       <c r="J68" s="1" t="n">
         <f aca="false">tblJoueurs!$B68</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K68" s="1" t="str">
         <f aca="false">tblJoueurs!$D68 &amp; " " &amp;tblJoueurs!$C68</f>
-        <v>Éric Caron-Malenfant</v>
+        <v>Tony Labillois</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B69" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C69" s="0" t="s">
+      <c r="A69" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B69" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D69" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F69" s="0" t="s">
+      <c r="E69" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G69" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H69" s="0" t="n">
-        <v>3</v>
+      <c r="G69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H69" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="I69" s="1" t="n">
         <f aca="false">tblJoueurs!$A69</f>
@@ -4946,37 +4949,37 @@
       </c>
       <c r="J69" s="1" t="n">
         <f aca="false">tblJoueurs!$B69</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K69" s="1" t="str">
         <f aca="false">tblJoueurs!$D69 &amp; " " &amp;tblJoueurs!$C69</f>
-        <v>Pierre Galarneau</v>
+        <v>Éric Caron-Malenfant</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B70" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C70" s="0" t="s">
+      <c r="A70" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B70" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D70" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G70" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H70" s="0" t="n">
-        <v>0</v>
+      <c r="D70" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G70" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H70" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I70" s="1" t="n">
         <f aca="false">tblJoueurs!$A70</f>
@@ -4984,36 +4987,36 @@
       </c>
       <c r="J70" s="1" t="n">
         <f aca="false">tblJoueurs!$B70</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K70" s="1" t="str">
         <f aca="false">tblJoueurs!$D70 &amp; " " &amp;tblJoueurs!$C70</f>
-        <v>Félix Labrecque-Synnott</v>
+        <v>Pierre Galarneau</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B71" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C71" s="0" t="s">
+      <c r="A71" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B71" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D71" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F71" s="0" t="s">
+      <c r="E71" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F71" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G71" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H71" s="0" t="n">
+      <c r="G71" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H71" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I71" s="1" t="n">
@@ -5022,36 +5025,36 @@
       </c>
       <c r="J71" s="1" t="n">
         <f aca="false">tblJoueurs!$B71</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K71" s="1" t="str">
         <f aca="false">tblJoueurs!$D71 &amp; " " &amp;tblJoueurs!$C71</f>
-        <v>Danielle Turpin</v>
+        <v>Félix Labrecque-Synnott</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B72" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="F72" s="0" t="s">
+      <c r="A72" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B72" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G72" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H72" s="0" t="n">
+      <c r="G72" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H72" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I72" s="1" t="n">
@@ -5060,36 +5063,36 @@
       </c>
       <c r="J72" s="1" t="n">
         <f aca="false">tblJoueurs!$B72</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K72" s="1" t="str">
         <f aca="false">tblJoueurs!$D72 &amp; " " &amp;tblJoueurs!$C72</f>
-        <v>James Falconer</v>
+        <v>Absent Absent</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B73" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="F73" s="0" t="s">
+      <c r="A73" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B73" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G73" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H73" s="0" t="n">
+      <c r="G73" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H73" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I73" s="1" t="n">
@@ -5098,36 +5101,36 @@
       </c>
       <c r="J73" s="1" t="n">
         <f aca="false">tblJoueurs!$B73</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K73" s="1" t="str">
         <f aca="false">tblJoueurs!$D73 &amp; " " &amp;tblJoueurs!$C73</f>
-        <v>Absent Absent</v>
+        <v>Catherine NA</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B74" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="C74" s="0" t="s">
+      <c r="A74" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B74" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D74" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F74" s="0" t="s">
+      <c r="D74" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F74" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G74" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H74" s="0" t="n">
+      <c r="G74" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H74" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I74" s="1" t="n">
@@ -5136,36 +5139,36 @@
       </c>
       <c r="J74" s="1" t="n">
         <f aca="false">tblJoueurs!$B74</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K74" s="1" t="str">
         <f aca="false">tblJoueurs!$D74 &amp; " " &amp;tblJoueurs!$C74</f>
-        <v>Catherine NA</v>
+        <v>Louis NA</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B75" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="F75" s="0" t="s">
+      <c r="A75" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B75" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G75" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H75" s="0" t="n">
+      <c r="G75" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H75" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I75" s="1" t="n">
@@ -5174,36 +5177,36 @@
       </c>
       <c r="J75" s="1" t="n">
         <f aca="false">tblJoueurs!$B75</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K75" s="1" t="str">
         <f aca="false">tblJoueurs!$D75 &amp; " " &amp;tblJoueurs!$C75</f>
-        <v>Louis NA</v>
+        <v>Étienne Lemyre (Faciles)</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B76" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="F76" s="0" t="s">
+      <c r="A76" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B76" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F76" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G76" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H76" s="0" t="n">
+      <c r="G76" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H76" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I76" s="1" t="n">
@@ -5212,36 +5215,36 @@
       </c>
       <c r="J76" s="1" t="n">
         <f aca="false">tblJoueurs!$B76</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K76" s="1" t="str">
         <f aca="false">tblJoueurs!$D76 &amp; " " &amp;tblJoueurs!$C76</f>
-        <v>Étienne Lemyre (Faciles)</v>
+        <v>Élizabeth LeBlanc</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B77" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="F77" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G77" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H77" s="0" t="n">
+      <c r="A77" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B77" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I77" s="1" t="n">
@@ -5250,49 +5253,25 @@
       </c>
       <c r="J77" s="1" t="n">
         <f aca="false">tblJoueurs!$B77</f>
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="K77" s="1" t="str">
         <f aca="false">tblJoueurs!$D77 &amp; " " &amp;tblJoueurs!$C77</f>
-        <v>Élizabeth LeBlanc</v>
+        <v>NA Les Faciles à cuire</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B78" s="0" t="n">
-        <v>99</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F78" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G78" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H78" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="I78" s="1" t="n">
         <f aca="false">tblJoueurs!$A78</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J78" s="1" t="n">
         <f aca="false">tblJoueurs!$B78</f>
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="K78" s="1" t="str">
         <f aca="false">tblJoueurs!$D78 &amp; " " &amp;tblJoueurs!$C78</f>
-        <v>NA Les Faciles à cuire</v>
+        <v> </v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5377,7 +5356,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.57"/>
@@ -5474,13 +5453,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>47</v>
@@ -5526,13 +5505,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>47</v>
@@ -5607,10 +5586,10 @@
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>47</v>
@@ -5656,13 +5635,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>47</v>
@@ -5682,13 +5661,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>37</v>
@@ -5708,13 +5687,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>47</v>
@@ -5734,13 +5713,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>47</v>
@@ -5760,13 +5739,13 @@
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>47</v>
@@ -6462,13 +6441,13 @@
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>34</v>
@@ -6488,7 +6467,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>45</v>
@@ -6514,13 +6493,13 @@
         <v>3</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>37</v>
@@ -6540,13 +6519,13 @@
         <v>4</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>37</v>
@@ -6566,13 +6545,13 @@
         <v>5</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>47</v>
@@ -6592,13 +6571,13 @@
         <v>6</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>47</v>
@@ -6644,13 +6623,13 @@
         <v>8</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>47</v>
@@ -6696,7 +6675,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>96</v>
@@ -6722,13 +6701,13 @@
         <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>47</v>
@@ -6748,13 +6727,13 @@
         <v>3</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>37</v>
@@ -6774,13 +6753,13 @@
         <v>2</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>37</v>
@@ -6800,13 +6779,13 @@
         <v>6</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>47</v>
@@ -6878,13 +6857,13 @@
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>34</v>
@@ -6904,13 +6883,13 @@
         <v>2</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>37</v>
@@ -6930,13 +6909,13 @@
         <v>3</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>37</v>
@@ -6956,7 +6935,7 @@
         <v>4</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>75</v>
@@ -6982,13 +6961,13 @@
         <v>5</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>47</v>
@@ -7216,13 +7195,13 @@
         <v>12</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>47</v>
@@ -7242,7 +7221,7 @@
         <v>11</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>77</v>
@@ -7268,13 +7247,13 @@
         <v>12</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Parties 3 et 4
</commit_message>
<xml_diff>
--- a/Saison24/DonnéesCSV/Saisie des points.xlsx
+++ b/Saison24/DonnéesCSV/Saisie des points.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Saisie" sheetId="1" state="visible" r:id="rId3"/>
@@ -43,61 +43,61 @@
     <t xml:space="preserve">Équipe A</t>
   </si>
   <si>
+    <t xml:space="preserve">Les 12e meilleurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoPartie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoÉquipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoJoueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Équipe B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les Bons Perdants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copie avec les bonnes colonnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NomÉquipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PosFinale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carillon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoÉquipe2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les Génies de la traduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les érudits en gerbe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les Herbizarres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les Méthos précieux</t>
+  </si>
+  <si>
     <t xml:space="preserve">Les Faciles à cuire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoPartie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoÉquipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoJoueur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Équipe B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les érudits en gerbe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copie avec les bonnes colonnes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomÉquipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PosFinale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carillon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoÉquipe2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Génies de la traduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Bons Perdants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Herbizarres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Méthos précieux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les 12e meilleurs</t>
   </si>
   <si>
     <t xml:space="preserve">NomJoueur</t>
@@ -734,20 +734,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblÉquipes" displayName="tblÉquipes" ref="A1:E8" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E8"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="NoÉquipe"/>
-    <tableColumn id="2" name="NomÉquipe"/>
-    <tableColumn id="3" name="PosFinale"/>
-    <tableColumn id="4" name="Carillon"/>
-    <tableColumn id="5" name="NoÉquipe2"/>
-  </tableColumns>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblJoueurs" displayName="tblJoueurs" ref="A1:K82" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblJoueurs" displayName="tblJoueurs" ref="A1:K82" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:K82"/>
   <tableColumns count="11">
     <tableColumn id="1" name="NoÉquipe"/>
@@ -761,6 +748,19 @@
     <tableColumn id="9" name="NoÉquipe2"/>
     <tableColumn id="10" name="NoJoueur2"/>
     <tableColumn id="11" name="Nom complet"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblÉquipes" displayName="tblÉquipes" ref="A1:E8" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E8"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="NoÉquipe"/>
+    <tableColumn id="2" name="NomÉquipe"/>
+    <tableColumn id="3" name="PosFinale"/>
+    <tableColumn id="4" name="Carillon"/>
+    <tableColumn id="5" name="NoÉquipe2"/>
   </tableColumns>
 </table>
 </file>
@@ -878,8 +878,8 @@
   </sheetPr>
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -916,7 +916,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,7 +928,7 @@
       </c>
       <c r="C3" s="1" t="n">
         <f aca="false">VLOOKUP(B3,tblÉquipes!$B$1:$E$8,4,FALSE())</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>6</v>
@@ -952,60 +952,60 @@
       </c>
       <c r="C4" s="1" t="n">
         <f aca="false">VLOOKUP(B4,tblÉquipes!$B$1:$E$8,4,FALSE())</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false" t="array" ref="F4:I13">_xlfn._xlws.FILTER(F18:I45,I18:I45&gt;0)</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="K4" s="1" t="str">
         <f aca="false">F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4</f>
-        <v>22,3,1,120</v>
+        <v>4,2,2,50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="1" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="K5" s="1" t="str">
         <f aca="false">F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5</f>
-        <v>22,3,2,50</v>
+        <v>4,2,4,80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F6" s="1" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="K6" s="1" t="str">
         <f aca="false">F6&amp;","&amp;G6&amp;","&amp;H6&amp;","&amp;I6</f>
-        <v>22,3,3,70</v>
+        <v>4,2,7,25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,214 +1022,212 @@
         <v>9</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="K7" s="1" t="str">
         <f aca="false">F7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7</f>
-        <v>22,3,4,50</v>
+        <v>4,2,9,70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <f aca="false" t="array" ref="A8:C30">_xlfn._xlws.FILTER(tblJoueurs!I:K,(tblJoueurs!I:I=$C$3)+(tblJoueurs!I:I=$C$4),"")</f>
-        <v>3</v>
+        <f aca="false" t="array" ref="A8:C32">_xlfn._xlws.FILTER(tblJoueurs!I:K,(tblJoueurs!I:I=$C$3)+(tblJoueurs!I:I=$C$4),"")</f>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="str">
-        <v>Mark Switzer</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>120</v>
-      </c>
+        <v>Steeve Boisvert</v>
+      </c>
+      <c r="D8" s="5"/>
       <c r="F8" s="1" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>99</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="K8" s="1" t="str">
         <f aca="false">F8&amp;","&amp;G8&amp;","&amp;H8&amp;","&amp;I8</f>
-        <v>22,3,99,10</v>
+        <v>4,2,99,30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="str">
-        <v>Pierre Parent</v>
+        <v>Samuel Perreault</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>50</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="K9" s="1" t="str">
         <f aca="false">F9&amp;","&amp;G9&amp;","&amp;H9&amp;","&amp;I9</f>
-        <v>22,7,1,100</v>
+        <v>4,6,1,130</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="str">
-        <v>François Rivest</v>
-      </c>
-      <c r="D10" s="5" t="n">
-        <v>70</v>
-      </c>
+        <v>Jonathan Baillargeon</v>
+      </c>
+      <c r="D10" s="5"/>
       <c r="F10" s="1" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="K10" s="1" t="str">
         <f aca="false">F10&amp;","&amp;G10&amp;","&amp;H10&amp;","&amp;I10</f>
-        <v>22,7,2,35</v>
+        <v>4,6,2,65</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C11" s="1" t="str">
-        <v>André Delage</v>
+        <v>Vincent Hardy</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="K11" s="1" t="str">
         <f aca="false">F11&amp;","&amp;G11&amp;","&amp;H11&amp;","&amp;I11</f>
-        <v>22,7,3,120</v>
+        <v>4,6,4,140</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="str">
-        <v>Louise Maheux</v>
+        <v>Nicole Paquin</v>
       </c>
       <c r="D12" s="5"/>
       <c r="F12" s="1" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="K12" s="1" t="str">
         <f aca="false">F12&amp;","&amp;G12&amp;","&amp;H12&amp;","&amp;I12</f>
-        <v>22,7,4,85</v>
+        <v>4,6,6,30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="str">
-        <v>Yanick Aubé</v>
+        <v>Franklin Assoumou</v>
       </c>
       <c r="D13" s="5"/>
       <c r="F13" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="G13" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H13" s="1" t="e">
-        <v>#N/A</v>
+        <v>4</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>99</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="K13" s="1" t="e">
+        <v>10</v>
+      </c>
+      <c r="K13" s="1" t="str">
         <f aca="false">F13&amp;","&amp;G13&amp;","&amp;H13&amp;","&amp;I13</f>
-        <v>#N/A</v>
+        <v>4,6,99,10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="str">
-        <v>Jean-Michel M.</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>Marie-Hélène Sarrasin</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>8</v>
@@ -1241,16 +1239,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="str">
-        <v>NA Les érudits en gerbe</v>
+        <v>Vincent Parenteau</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>13</v>
@@ -1260,17 +1258,15 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1" t="str">
-        <v>Philippe Bérubé</v>
-      </c>
-      <c r="D17" s="5" t="n">
-        <v>100</v>
-      </c>
+        <v>Cindy Lecavalier</v>
+      </c>
+      <c r="D17" s="5"/>
       <c r="F17" s="4" t="s">
         <v>6</v>
       </c>
@@ -1286,24 +1282,24 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="C18" s="1" t="str">
-        <v>Tony Labillois</v>
+        <v>NA Les Bons Perdants</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G18" s="1" t="n">
         <f aca="false">A8</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18" s="1" t="n">
         <f aca="false">B8</f>
@@ -1311,29 +1307,29 @@
       </c>
       <c r="I18" s="1" t="n">
         <f aca="false">D8</f>
-        <v>120</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1" t="str">
-        <v>Éric Caron-Malenfant</v>
+        <v>Stéphane Mongeau</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G19" s="1" t="n">
         <f aca="false">A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H19" s="1" t="n">
         <f aca="false">B9</f>
@@ -1346,24 +1342,24 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C20" s="1" t="str">
-        <v>Pierre Galarneau</v>
+        <v>Pierre-Olivier Julien</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F20" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G20" s="1" t="n">
         <f aca="false">A10</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20" s="1" t="n">
         <f aca="false">B10</f>
@@ -1371,27 +1367,27 @@
       </c>
       <c r="I20" s="1" t="n">
         <f aca="false">D10</f>
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1" t="str">
-        <v>Félix Labrecque-Synnott</v>
+        <v>Julien Bérard-Chagnon</v>
       </c>
       <c r="D21" s="5"/>
       <c r="F21" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G21" s="1" t="n">
         <f aca="false">A11</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H21" s="1" t="n">
         <f aca="false">B11</f>
@@ -1399,27 +1395,29 @@
       </c>
       <c r="I21" s="1" t="n">
         <f aca="false">D11</f>
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1" t="str">
-        <v>Absent Absent</v>
-      </c>
-      <c r="D22" s="5"/>
+        <v>Patrick Charbonneau</v>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>140</v>
+      </c>
       <c r="F22" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G22" s="1" t="n">
         <f aca="false">A12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22" s="1" t="n">
         <f aca="false">B12</f>
@@ -1432,22 +1430,22 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1" t="str">
-        <v>Catherine NA</v>
+        <v>Keven Bosa</v>
       </c>
       <c r="D23" s="5"/>
       <c r="F23" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G23" s="1" t="n">
         <f aca="false">A13</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H23" s="1" t="n">
         <f aca="false">B13</f>
@@ -1460,22 +1458,24 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1" t="str">
-        <v>Louis NA</v>
-      </c>
-      <c r="D24" s="5"/>
+        <v>Étienne Rassart</v>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>30</v>
+      </c>
       <c r="F24" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G24" s="1" t="n">
         <f aca="false">A14</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">B14</f>
@@ -1483,27 +1483,27 @@
       </c>
       <c r="I24" s="1" t="n">
         <f aca="false">D14</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B25" s="1" t="n">
-        <v>11</v>
-      </c>
       <c r="C25" s="1" t="str">
-        <v>Étienne Lemyre (Faciles)</v>
+        <v>Daphné Allard Gervais</v>
       </c>
       <c r="D25" s="5"/>
       <c r="F25" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G25" s="1" t="n">
         <f aca="false">A15</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">B15</f>
@@ -1516,159 +1516,168 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C26" s="1" t="str">
-        <v>Élizabeth LeBlanc</v>
+        <v>Emy Bourdages</v>
       </c>
       <c r="D26" s="5"/>
       <c r="F26" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G26" s="1" t="n">
         <f aca="false">A16</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">B16</f>
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="I26" s="1" t="n">
         <f aca="false">D16</f>
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="C27" s="1" t="str">
-        <v>NA Les Faciles à cuire</v>
+        <v>David Binet</v>
       </c>
       <c r="D27" s="5"/>
       <c r="F27" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G27" s="1" t="n">
         <f aca="false">A17</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H27" s="1" t="n">
         <f aca="false">B17</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I27" s="1" t="n">
         <f aca="false">D17</f>
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B28" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C28" s="1" t="e">
-        <v>#N/A</v>
+      <c r="A28" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <v>Absent Absent</v>
       </c>
       <c r="D28" s="5"/>
       <c r="F28" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G28" s="1" t="n">
         <f aca="false">A18</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H28" s="1" t="n">
         <f aca="false">B18</f>
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="I28" s="1" t="n">
         <f aca="false">D18</f>
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B29" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C29" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D29" s="5" t="n">
-        <v>40</v>
-      </c>
+      <c r="A29" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C29" s="1" t="str">
+        <v>François Sergerie</v>
+      </c>
+      <c r="D29" s="5"/>
       <c r="F29" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G29" s="1" t="n">
         <f aca="false">A19</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H29" s="1" t="n">
         <f aca="false">B19</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I29" s="1" t="n">
         <f aca="false">D19</f>
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B30" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C30" s="1" t="e">
-        <v>#N/A</v>
+      <c r="A30" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <v>Arnaud Bouchard-Santerre</v>
       </c>
       <c r="D30" s="5"/>
       <c r="F30" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G30" s="1" t="n">
         <f aca="false">A20</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H30" s="1" t="n">
         <f aca="false">B20</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I30" s="1" t="n">
         <f aca="false">D20</f>
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="5"/>
+      <c r="A31" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="C31" s="1" t="str">
+        <v>NA Les 12e meilleurs</v>
+      </c>
+      <c r="D31" s="5" t="n">
+        <v>10</v>
+      </c>
       <c r="F31" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G31" s="1" t="n">
         <f aca="false">A21</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H31" s="1" t="n">
         <f aca="false">B21</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I31" s="1" t="n">
         <f aca="false">D21</f>
@@ -1676,37 +1685,46 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B32" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C32" s="1" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="D32" s="5"/>
       <c r="F32" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G32" s="1" t="n">
         <f aca="false">A22</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H32" s="1" t="n">
         <f aca="false">B22</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I32" s="1" t="n">
         <f aca="false">D22</f>
-        <v>0</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="5"/>
       <c r="F33" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G33" s="1" t="n">
         <f aca="false">A23</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H33" s="1" t="n">
         <f aca="false">B23</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I33" s="1" t="n">
         <f aca="false">D23</f>
@@ -1716,33 +1734,33 @@
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F34" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G34" s="1" t="n">
         <f aca="false">A24</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H34" s="1" t="n">
         <f aca="false">B24</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I34" s="1" t="n">
         <f aca="false">D24</f>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G35" s="1" t="n">
         <f aca="false">A25</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H35" s="1" t="n">
         <f aca="false">B25</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I35" s="1" t="n">
         <f aca="false">D25</f>
@@ -1752,15 +1770,15 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F36" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G36" s="1" t="n">
         <f aca="false">A26</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">B26</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I36" s="1" t="n">
         <f aca="false">D26</f>
@@ -1770,15 +1788,15 @@
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F37" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G37" s="1" t="n">
         <f aca="false">A27</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">B27</f>
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="I37" s="1" t="n">
         <f aca="false">D27</f>
@@ -1788,15 +1806,15 @@
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F38" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
-      </c>
-      <c r="G38" s="1" t="e">
+        <v>4</v>
+      </c>
+      <c r="G38" s="1" t="n">
         <f aca="false">A28</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H38" s="1" t="e">
+        <v>6</v>
+      </c>
+      <c r="H38" s="1" t="n">
         <f aca="false">B28</f>
-        <v>#N/A</v>
+        <v>10</v>
       </c>
       <c r="I38" s="1" t="n">
         <f aca="false">D28</f>
@@ -1806,33 +1824,33 @@
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F39" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
-      </c>
-      <c r="G39" s="1" t="e">
+        <v>4</v>
+      </c>
+      <c r="G39" s="1" t="n">
         <f aca="false">A29</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H39" s="1" t="e">
+        <v>6</v>
+      </c>
+      <c r="H39" s="1" t="n">
         <f aca="false">B29</f>
-        <v>#N/A</v>
+        <v>11</v>
       </c>
       <c r="I39" s="1" t="n">
         <f aca="false">D29</f>
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F40" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
-      </c>
-      <c r="G40" s="1" t="e">
+        <v>4</v>
+      </c>
+      <c r="G40" s="1" t="n">
         <f aca="false">A30</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H40" s="1" t="e">
+        <v>6</v>
+      </c>
+      <c r="H40" s="1" t="n">
         <f aca="false">B30</f>
-        <v>#N/A</v>
+        <v>12</v>
       </c>
       <c r="I40" s="1" t="n">
         <f aca="false">D30</f>
@@ -1842,33 +1860,33 @@
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F41" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G41" s="1" t="n">
         <f aca="false">A31</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H41" s="1" t="n">
         <f aca="false">B31</f>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="I41" s="1" t="n">
         <f aca="false">D31</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F42" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
-      </c>
-      <c r="G42" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G42" s="1" t="e">
         <f aca="false">A32</f>
-        <v>0</v>
-      </c>
-      <c r="H42" s="1" t="n">
+        <v>#N/A</v>
+      </c>
+      <c r="H42" s="1" t="e">
         <f aca="false">B32</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="I42" s="1" t="n">
         <f aca="false">D32</f>
@@ -1878,7 +1896,7 @@
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F43" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G43" s="1" t="n">
         <f aca="false">A33</f>
@@ -1896,7 +1914,7 @@
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F44" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G44" s="1" t="n">
         <f aca="false">A34</f>
@@ -1914,7 +1932,7 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F45" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G45" s="1" t="n">
         <f aca="false">A35</f>
@@ -2010,7 +2028,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -2028,7 +2046,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
@@ -2082,7 +2100,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
@@ -2100,7 +2118,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -2134,8 +2152,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3142,13 +3160,13 @@
         <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>54</v>
@@ -3520,13 +3538,13 @@
         <v>99</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>54</v>
@@ -4812,13 +4830,13 @@
         <v>99</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>54</v>
@@ -5230,13 +5248,13 @@
         <v>99</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>54</v>
@@ -5999,13 +6017,13 @@
         <v>99</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>54</v>
@@ -6181,13 +6199,13 @@
         <v>99</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>54</v>
@@ -6831,13 +6849,13 @@
         <v>99</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>54</v>
@@ -7013,13 +7031,13 @@
         <v>99</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Parties 7 et 8
</commit_message>
<xml_diff>
--- a/Saison24/DonnéesCSV/Saisie des points.xlsx
+++ b/Saison24/DonnéesCSV/Saisie des points.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Saisie" sheetId="1" state="visible" r:id="rId3"/>
@@ -43,58 +43,58 @@
     <t xml:space="preserve">Équipe A</t>
   </si>
   <si>
+    <t xml:space="preserve">Les Herbizarres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoPartie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoÉquipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoJoueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Équipe B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les Méthos précieux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copie avec les bonnes colonnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NomÉquipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PosFinale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carillon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoÉquipe2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les Génies de la traduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les Bons Perdants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les érudits en gerbe</t>
+  </si>
+  <si>
     <t xml:space="preserve">Les 12e meilleurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoPartie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoÉquipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoJoueur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Équipe B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Bons Perdants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copie avec les bonnes colonnes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomÉquipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PosFinale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carillon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoÉquipe2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Génies de la traduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les érudits en gerbe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Herbizarres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Méthos précieux</t>
   </si>
   <si>
     <t xml:space="preserve">Les Faciles à cuire</t>
@@ -884,8 +884,8 @@
   </sheetPr>
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -922,7 +922,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,7 +934,7 @@
       </c>
       <c r="C3" s="1" t="n">
         <f aca="false">VLOOKUP(B3,tblÉquipes!$B$1:$E$8,4,FALSE())</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>6</v>
@@ -958,60 +958,60 @@
       </c>
       <c r="C4" s="1" t="n">
         <f aca="false">VLOOKUP(B4,tblÉquipes!$B$1:$E$8,4,FALSE())</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false" t="array" ref="F4:I13">_xlfn._xlws.FILTER(F18:I45,I18:I45&gt;0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="K4" s="1" t="str">
         <f aca="false">F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4</f>
-        <v>4,2,2,50</v>
+        <v>6,4,1,115</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="K5" s="1" t="str">
         <f aca="false">F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5</f>
-        <v>4,2,4,80</v>
+        <v>6,4,2,70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F6" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="K6" s="1" t="str">
         <f aca="false">F6&amp;","&amp;G6&amp;","&amp;H6&amp;","&amp;I6</f>
-        <v>4,2,7,25</v>
+        <v>6,4,3,70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,234 +1028,232 @@
         <v>9</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="K7" s="1" t="str">
         <f aca="false">F7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7</f>
-        <v>4,2,9,70</v>
+        <v>6,4,11,20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <f aca="false" t="array" ref="A8:C32">_xlfn._xlws.FILTER(tblJoueurs!I:K,(tblJoueurs!I:I=$C$3)+(tblJoueurs!I:I=$C$4),"")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="str">
-        <v>Steeve Boisvert</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>Sébastien Landry</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>115</v>
+      </c>
       <c r="F8" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>99</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K8" s="1" t="str">
         <f aca="false">F8&amp;","&amp;G8&amp;","&amp;H8&amp;","&amp;I8</f>
-        <v>4,2,99,30</v>
+        <v>6,4,99,20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="str">
-        <v>Samuel Perreault</v>
+        <v>Frédéric Bédard</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="K9" s="1" t="str">
         <f aca="false">F9&amp;","&amp;G9&amp;","&amp;H9&amp;","&amp;I9</f>
-        <v>4,6,1,130</v>
+        <v>6,5,1,80</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="str">
-        <v>Jonathan Baillargeon</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>Geneviève Ouellet</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>70</v>
+      </c>
       <c r="F10" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K10" s="1" t="str">
         <f aca="false">F10&amp;","&amp;G10&amp;","&amp;H10&amp;","&amp;I10</f>
-        <v>4,6,2,65</v>
+        <v>6,5,2,60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C11" s="1" t="str">
-        <v>Vincent Hardy</v>
-      </c>
-      <c r="D11" s="5" t="n">
-        <v>80</v>
-      </c>
+        <v>Samuel Vézina</v>
+      </c>
+      <c r="D11" s="5"/>
       <c r="F11" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="K11" s="1" t="str">
         <f aca="false">F11&amp;","&amp;G11&amp;","&amp;H11&amp;","&amp;I11</f>
-        <v>4,6,4,140</v>
+        <v>6,5,3,40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="str">
-        <v>Nicole Paquin</v>
+        <v>Jean-Dominique Morency</v>
       </c>
       <c r="D12" s="5"/>
       <c r="F12" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K12" s="1" t="str">
         <f aca="false">F12&amp;","&amp;G12&amp;","&amp;H12&amp;","&amp;I12</f>
-        <v>4,6,6,30</v>
+        <v>6,5,4,40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="str">
-        <v>Franklin Assoumou</v>
+        <v>Stéphane Martineau</v>
       </c>
       <c r="D13" s="5"/>
       <c r="F13" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>99</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="K13" s="1" t="str">
         <f aca="false">F13&amp;","&amp;G13&amp;","&amp;H13&amp;","&amp;I13</f>
-        <v>4,6,99,10</v>
+        <v>6,5,99,40</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="str">
-        <v>Marie-Hélène Sarrasin</v>
-      </c>
-      <c r="D14" s="5" t="n">
-        <v>25</v>
-      </c>
+        <v>Michel Parenteau</v>
+      </c>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="str">
-        <v>Absent Absent</v>
+        <v>Caroline Pelletier</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C16" s="1" t="str">
-        <v>Vincent Parenteau</v>
-      </c>
-      <c r="D16" s="5" t="n">
-        <v>70</v>
-      </c>
+        <v>Absent Absent</v>
+      </c>
+      <c r="D16" s="5"/>
       <c r="F16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1264,13 +1262,13 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>10</v>
       </c>
       <c r="C17" s="1" t="str">
-        <v>Cindy Lecavalier</v>
+        <v>Sylvain Coulombe</v>
       </c>
       <c r="D17" s="5"/>
       <c r="F17" s="4" t="s">
@@ -1288,24 +1286,24 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="str">
-        <v>NA Les Bons Perdants</v>
+        <v>Francis Demers</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G18" s="1" t="n">
         <f aca="false">A8</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H18" s="1" t="n">
         <f aca="false">B8</f>
@@ -1313,29 +1311,29 @@
       </c>
       <c r="I18" s="1" t="n">
         <f aca="false">D8</f>
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="C19" s="1" t="str">
-        <v>Stéphane Mongeau</v>
+        <v>NA Les Herbizarres</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G19" s="1" t="n">
         <f aca="false">A9</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H19" s="1" t="n">
         <f aca="false">B9</f>
@@ -1343,29 +1341,29 @@
       </c>
       <c r="I19" s="1" t="n">
         <f aca="false">D9</f>
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1" t="str">
-        <v>Pierre-Olivier Julien</v>
+        <v>Bruno Lapierre</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F20" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G20" s="1" t="n">
         <f aca="false">A10</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H20" s="1" t="n">
         <f aca="false">B10</f>
@@ -1373,27 +1371,29 @@
       </c>
       <c r="I20" s="1" t="n">
         <f aca="false">D10</f>
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1" t="str">
-        <v>Julien Bérard-Chagnon</v>
-      </c>
-      <c r="D21" s="5"/>
+        <v>Julie Bernier</v>
+      </c>
+      <c r="D21" s="5" t="n">
+        <v>60</v>
+      </c>
       <c r="F21" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G21" s="1" t="n">
         <f aca="false">A11</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H21" s="1" t="n">
         <f aca="false">B11</f>
@@ -1401,29 +1401,29 @@
       </c>
       <c r="I21" s="1" t="n">
         <f aca="false">D11</f>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1" t="str">
-        <v>Patrick Charbonneau</v>
+        <v>Sylvain Perron</v>
       </c>
       <c r="D22" s="5" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="F22" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G22" s="1" t="n">
         <f aca="false">A12</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H22" s="1" t="n">
         <f aca="false">B12</f>
@@ -1436,22 +1436,24 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1" t="str">
-        <v>Keven Bosa</v>
-      </c>
-      <c r="D23" s="5"/>
+        <v>Martin Sirois</v>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>40</v>
+      </c>
       <c r="F23" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G23" s="1" t="n">
         <f aca="false">A13</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H23" s="1" t="n">
         <f aca="false">B13</f>
@@ -1464,24 +1466,22 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="1" t="str">
-        <v>Étienne Lemyre</v>
-      </c>
-      <c r="D24" s="5" t="n">
-        <v>30</v>
-      </c>
+        <v>Didier Garriguet</v>
+      </c>
+      <c r="D24" s="5"/>
       <c r="F24" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G24" s="1" t="n">
         <f aca="false">A14</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">B14</f>
@@ -1489,27 +1489,27 @@
       </c>
       <c r="I24" s="1" t="n">
         <f aca="false">D14</f>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1" t="str">
-        <v>Daphné Allard Gervais</v>
+        <v>Jean-Sébastien Provencal</v>
       </c>
       <c r="D25" s="5"/>
       <c r="F25" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G25" s="1" t="n">
         <f aca="false">A15</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">B15</f>
@@ -1522,22 +1522,22 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" s="1" t="str">
-        <v>Emy Bourdages</v>
+        <v>Absent Absent</v>
       </c>
       <c r="D26" s="5"/>
       <c r="F26" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G26" s="1" t="n">
         <f aca="false">A16</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">B16</f>
@@ -1545,27 +1545,27 @@
       </c>
       <c r="I26" s="1" t="n">
         <f aca="false">D16</f>
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="1" t="str">
-        <v>David Binet</v>
+        <v>Marlène Savard</v>
       </c>
       <c r="D27" s="5"/>
       <c r="F27" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G27" s="1" t="n">
         <f aca="false">A17</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H27" s="1" t="n">
         <f aca="false">B17</f>
@@ -1578,116 +1578,116 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" s="1" t="str">
-        <v>Absent Absent</v>
+        <v>François Lavoie</v>
       </c>
       <c r="D28" s="5"/>
       <c r="F28" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G28" s="1" t="n">
         <f aca="false">A18</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H28" s="1" t="n">
         <f aca="false">B18</f>
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="I28" s="1" t="n">
         <f aca="false">D18</f>
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="C29" s="1" t="str">
-        <v>François Sergerie</v>
-      </c>
-      <c r="D29" s="5"/>
+        <v>NA Les Méthos précieux</v>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>40</v>
+      </c>
       <c r="F29" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G29" s="1" t="n">
         <f aca="false">A19</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H29" s="1" t="n">
         <f aca="false">B19</f>
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="I29" s="1" t="n">
         <f aca="false">D19</f>
-        <v>130</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B30" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="C30" s="1" t="str">
-        <v>Arnaud Bouchard-Santerre</v>
+      <c r="A30" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B30" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C30" s="1" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D30" s="5"/>
       <c r="F30" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G30" s="1" t="n">
         <f aca="false">A20</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H30" s="1" t="n">
         <f aca="false">B20</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30" s="1" t="n">
         <f aca="false">D20</f>
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B31" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="C31" s="1" t="str">
-        <v>NA Les 12e meilleurs</v>
-      </c>
-      <c r="D31" s="5" t="n">
-        <v>10</v>
-      </c>
+      <c r="A31" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B31" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C31" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D31" s="5"/>
       <c r="F31" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G31" s="1" t="n">
         <f aca="false">A21</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H31" s="1" t="n">
         <f aca="false">B21</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I31" s="1" t="n">
         <f aca="false">D21</f>
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,70 +1703,70 @@
       <c r="D32" s="5"/>
       <c r="F32" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G32" s="1" t="n">
         <f aca="false">A22</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H32" s="1" t="n">
         <f aca="false">B22</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I32" s="1" t="n">
         <f aca="false">D22</f>
-        <v>140</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="5"/>
       <c r="F33" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G33" s="1" t="n">
         <f aca="false">A23</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H33" s="1" t="n">
         <f aca="false">B23</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I33" s="1" t="n">
         <f aca="false">D23</f>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F34" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G34" s="1" t="n">
         <f aca="false">A24</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H34" s="1" t="n">
         <f aca="false">B24</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I34" s="1" t="n">
         <f aca="false">D24</f>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G35" s="1" t="n">
         <f aca="false">A25</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H35" s="1" t="n">
         <f aca="false">B25</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I35" s="1" t="n">
         <f aca="false">D25</f>
@@ -1776,15 +1776,15 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F36" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G36" s="1" t="n">
         <f aca="false">A26</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">B26</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I36" s="1" t="n">
         <f aca="false">D26</f>
@@ -1794,15 +1794,15 @@
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F37" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G37" s="1" t="n">
         <f aca="false">A27</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">B27</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I37" s="1" t="n">
         <f aca="false">D27</f>
@@ -1812,15 +1812,15 @@
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F38" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G38" s="1" t="n">
         <f aca="false">A28</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H38" s="1" t="n">
         <f aca="false">B28</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I38" s="1" t="n">
         <f aca="false">D28</f>
@@ -1830,33 +1830,33 @@
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F39" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G39" s="1" t="n">
         <f aca="false">A29</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H39" s="1" t="n">
         <f aca="false">B29</f>
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="I39" s="1" t="n">
         <f aca="false">D29</f>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F40" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
-      </c>
-      <c r="G40" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G40" s="1" t="e">
         <f aca="false">A30</f>
-        <v>6</v>
-      </c>
-      <c r="H40" s="1" t="n">
+        <v>#N/A</v>
+      </c>
+      <c r="H40" s="1" t="e">
         <f aca="false">B30</f>
-        <v>12</v>
+        <v>#N/A</v>
       </c>
       <c r="I40" s="1" t="n">
         <f aca="false">D30</f>
@@ -1866,25 +1866,25 @@
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F41" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
-      </c>
-      <c r="G41" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G41" s="1" t="e">
         <f aca="false">A31</f>
-        <v>6</v>
-      </c>
-      <c r="H41" s="1" t="n">
+        <v>#N/A</v>
+      </c>
+      <c r="H41" s="1" t="e">
         <f aca="false">B31</f>
-        <v>99</v>
+        <v>#N/A</v>
       </c>
       <c r="I41" s="1" t="n">
         <f aca="false">D31</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F42" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G42" s="1" t="e">
         <f aca="false">A32</f>
@@ -1902,7 +1902,7 @@
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F43" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G43" s="1" t="n">
         <f aca="false">A33</f>
@@ -1920,7 +1920,7 @@
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F44" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G44" s="1" t="n">
         <f aca="false">A34</f>
@@ -1938,7 +1938,7 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F45" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G45" s="1" t="n">
         <f aca="false">A35</f>
@@ -1982,7 +1982,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="topLeft" activeCell="I14" activeCellId="1" sqref="K4:K13 I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2034,7 +2034,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -2052,7 +2052,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
@@ -2070,7 +2070,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
@@ -2088,7 +2088,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>19</v>
@@ -2106,7 +2106,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
@@ -2158,8 +2158,8 @@
   </sheetPr>
   <dimension ref="A1:Q83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B43" activeCellId="1" sqref="K4:K13 B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3166,13 +3166,13 @@
         <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>54</v>
@@ -3544,13 +3544,13 @@
         <v>99</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>54</v>
@@ -4000,13 +4000,13 @@
         <v>99</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>54</v>
@@ -4380,13 +4380,13 @@
         <v>99</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>54</v>
@@ -4874,13 +4874,13 @@
         <v>99</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>54</v>
@@ -5414,7 +5414,7 @@
   <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="K4:K13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6060,13 +6060,13 @@
         <v>99</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>54</v>
@@ -6242,13 +6242,13 @@
         <v>99</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>54</v>
@@ -6476,13 +6476,13 @@
         <v>99</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>54</v>
@@ -6710,13 +6710,13 @@
         <v>99</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>54</v>
@@ -6892,13 +6892,13 @@
         <v>99</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Parties 9 et 10
</commit_message>
<xml_diff>
--- a/Saison24/DonnéesCSV/Saisie des points.xlsx
+++ b/Saison24/DonnéesCSV/Saisie des points.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="155">
   <si>
     <t xml:space="preserve">Saisi des points</t>
   </si>
@@ -43,60 +43,60 @@
     <t xml:space="preserve">Équipe A</t>
   </si>
   <si>
+    <t xml:space="preserve">Les Bons Perdants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoPartie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoÉquipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoJoueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Équipe B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les 12e meilleurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copie avec les bonnes colonnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NomÉquipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PosFinale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carillon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoÉquipe2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les Génies de la traduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les érudits en gerbe</t>
+  </si>
+  <si>
     <t xml:space="preserve">Les Herbizarres</t>
   </si>
   <si>
-    <t xml:space="preserve">NoPartie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoÉquipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoJoueur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Équipe B</t>
-  </si>
-  <si>
     <t xml:space="preserve">Les Méthos précieux</t>
   </si>
   <si>
-    <t xml:space="preserve">Nom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copie avec les bonnes colonnes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomÉquipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PosFinale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carillon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoÉquipe2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Génies de la traduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Bons Perdants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les érudits en gerbe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les 12e meilleurs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Les Faciles à cuire</t>
   </si>
   <si>
@@ -458,6 +458,12 @@
   </si>
   <si>
     <t xml:space="preserve">Félix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gilbert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yves</t>
   </si>
   <si>
     <t xml:space="preserve">Louis</t>
@@ -740,8 +746,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblJoueurs" displayName="tblJoueurs" ref="A1:K83" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K83"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblJoueurs" displayName="tblJoueurs" ref="A1:K84" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:K84"/>
   <tableColumns count="11">
     <tableColumn id="1" name="NoÉquipe"/>
     <tableColumn id="2" name="NoJoueur"/>
@@ -884,8 +890,8 @@
   </sheetPr>
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4:K13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K4:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -922,7 +928,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,7 +940,7 @@
       </c>
       <c r="C3" s="1" t="n">
         <f aca="false">VLOOKUP(B3,tblÉquipes!$B$1:$E$8,4,FALSE())</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>6</v>
@@ -958,60 +964,60 @@
       </c>
       <c r="C4" s="1" t="n">
         <f aca="false">VLOOKUP(B4,tblÉquipes!$B$1:$E$8,4,FALSE())</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false" t="array" ref="F4:I13">_xlfn._xlws.FILTER(F18:I45,I18:I45&gt;0)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>115</v>
+        <v>200</v>
       </c>
       <c r="K4" s="1" t="str">
         <f aca="false">F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4</f>
-        <v>6,4,1,115</v>
+        <v>5,2,1,200</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="K5" s="1" t="str">
         <f aca="false">F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5</f>
-        <v>6,4,2,70</v>
+        <v>5,2,4,95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F6" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="K6" s="1" t="str">
         <f aca="false">F6&amp;","&amp;G6&amp;","&amp;H6&amp;","&amp;I6</f>
-        <v>6,4,3,70</v>
+        <v>5,2,7,20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,232 +1034,234 @@
         <v>9</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="K7" s="1" t="str">
         <f aca="false">F7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7</f>
-        <v>6,4,11,20</v>
+        <v>5,2,9,50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <f aca="false" t="array" ref="A8:C32">_xlfn._xlws.FILTER(tblJoueurs!I:K,(tblJoueurs!I:I=$C$3)+(tblJoueurs!I:I=$C$4),"")</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="str">
-        <v>Sébastien Landry</v>
+        <v>Steeve Boisvert</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>115</v>
+        <v>200</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>99</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="K8" s="1" t="str">
         <f aca="false">F8&amp;","&amp;G8&amp;","&amp;H8&amp;","&amp;I8</f>
-        <v>6,4,99,20</v>
+        <v>5,2,99,50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="str">
-        <v>Frédéric Bédard</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>70</v>
-      </c>
+        <v>Samuel Perreault</v>
+      </c>
+      <c r="D9" s="5"/>
       <c r="F9" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="K9" s="1" t="str">
         <f aca="false">F9&amp;","&amp;G9&amp;","&amp;H9&amp;","&amp;I9</f>
-        <v>6,5,1,80</v>
+        <v>5,6,1,50</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="str">
-        <v>Geneviève Ouellet</v>
-      </c>
-      <c r="D10" s="5" t="n">
-        <v>70</v>
-      </c>
+        <v>Jonathan Baillargeon</v>
+      </c>
+      <c r="D10" s="5"/>
       <c r="F10" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K10" s="1" t="str">
         <f aca="false">F10&amp;","&amp;G10&amp;","&amp;H10&amp;","&amp;I10</f>
-        <v>6,5,2,60</v>
+        <v>5,6,2,30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C11" s="1" t="str">
-        <v>Samuel Vézina</v>
-      </c>
-      <c r="D11" s="5"/>
+        <v>Vincent Hardy</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>95</v>
+      </c>
       <c r="F11" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="K11" s="1" t="str">
         <f aca="false">F11&amp;","&amp;G11&amp;","&amp;H11&amp;","&amp;I11</f>
-        <v>6,5,3,40</v>
+        <v>5,6,4,60</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="str">
-        <v>Jean-Dominique Morency</v>
+        <v>Nicole Paquin</v>
       </c>
       <c r="D12" s="5"/>
       <c r="F12" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="K12" s="1" t="str">
         <f aca="false">F12&amp;","&amp;G12&amp;","&amp;H12&amp;","&amp;I12</f>
-        <v>6,5,4,40</v>
+        <v>5,6,6,10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="str">
-        <v>Stéphane Martineau</v>
+        <v>Franklin Assoumou</v>
       </c>
       <c r="D13" s="5"/>
       <c r="F13" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>99</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K13" s="1" t="str">
         <f aca="false">F13&amp;","&amp;G13&amp;","&amp;H13&amp;","&amp;I13</f>
-        <v>6,5,99,40</v>
+        <v>5,6,99,50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="str">
-        <v>Michel Parenteau</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>Marie-Hélène Sarrasin</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="str">
-        <v>Caroline Pelletier</v>
+        <v>Absent Absent</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C16" s="1" t="str">
-        <v>Absent Absent</v>
-      </c>
-      <c r="D16" s="5"/>
+        <v>Vincent Parenteau</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>50</v>
+      </c>
       <c r="F16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1262,13 +1270,13 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>10</v>
       </c>
       <c r="C17" s="1" t="str">
-        <v>Sylvain Coulombe</v>
+        <v>Cindy Lecavalier</v>
       </c>
       <c r="D17" s="5"/>
       <c r="F17" s="4" t="s">
@@ -1286,24 +1294,24 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="C18" s="1" t="str">
-        <v>Francis Demers</v>
+        <v>NA Les Bons Perdants</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G18" s="1" t="n">
         <f aca="false">A8</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H18" s="1" t="n">
         <f aca="false">B8</f>
@@ -1311,29 +1319,29 @@
       </c>
       <c r="I18" s="1" t="n">
         <f aca="false">D8</f>
-        <v>115</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1" t="str">
-        <v>NA Les Herbizarres</v>
+        <v>Stéphane Mongeau</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G19" s="1" t="n">
         <f aca="false">A9</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19" s="1" t="n">
         <f aca="false">B9</f>
@@ -1341,29 +1349,29 @@
       </c>
       <c r="I19" s="1" t="n">
         <f aca="false">D9</f>
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="1" t="str">
-        <v>Bruno Lapierre</v>
+        <v>Pierre-Olivier Julien</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="F20" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G20" s="1" t="n">
         <f aca="false">A10</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H20" s="1" t="n">
         <f aca="false">B10</f>
@@ -1371,29 +1379,27 @@
       </c>
       <c r="I20" s="1" t="n">
         <f aca="false">D10</f>
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1" t="str">
-        <v>Julie Bernier</v>
-      </c>
-      <c r="D21" s="5" t="n">
-        <v>60</v>
-      </c>
+        <v>Julien Bérard-Chagnon</v>
+      </c>
+      <c r="D21" s="5"/>
       <c r="F21" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G21" s="1" t="n">
         <f aca="false">A11</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H21" s="1" t="n">
         <f aca="false">B11</f>
@@ -1401,29 +1407,29 @@
       </c>
       <c r="I21" s="1" t="n">
         <f aca="false">D11</f>
-        <v>0</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1" t="str">
-        <v>Sylvain Perron</v>
+        <v>Patrick Charbonneau</v>
       </c>
       <c r="D22" s="5" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F22" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G22" s="1" t="n">
         <f aca="false">A12</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H22" s="1" t="n">
         <f aca="false">B12</f>
@@ -1436,24 +1442,22 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1" t="str">
-        <v>Martin Sirois</v>
-      </c>
-      <c r="D23" s="5" t="n">
-        <v>40</v>
-      </c>
+        <v>Keven Bosa</v>
+      </c>
+      <c r="D23" s="5"/>
       <c r="F23" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G23" s="1" t="n">
         <f aca="false">A13</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H23" s="1" t="n">
         <f aca="false">B13</f>
@@ -1466,22 +1470,24 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1" t="str">
-        <v>Didier Garriguet</v>
-      </c>
-      <c r="D24" s="5"/>
+        <v>Étienne Lemyre</v>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>10</v>
+      </c>
       <c r="F24" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G24" s="1" t="n">
         <f aca="false">A14</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">B14</f>
@@ -1489,27 +1495,27 @@
       </c>
       <c r="I24" s="1" t="n">
         <f aca="false">D14</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25" s="1" t="str">
-        <v>Jean-Sébastien Provencal</v>
+        <v>Daphné Allard Gervais</v>
       </c>
       <c r="D25" s="5"/>
       <c r="F25" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G25" s="1" t="n">
         <f aca="false">A15</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">B15</f>
@@ -1522,22 +1528,22 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C26" s="1" t="str">
-        <v>Absent Absent</v>
+        <v>Emy Bourdages</v>
       </c>
       <c r="D26" s="5"/>
       <c r="F26" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G26" s="1" t="n">
         <f aca="false">A16</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">B16</f>
@@ -1545,27 +1551,27 @@
       </c>
       <c r="I26" s="1" t="n">
         <f aca="false">D16</f>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27" s="1" t="str">
-        <v>Marlène Savard</v>
+        <v>David Binet</v>
       </c>
       <c r="D27" s="5"/>
       <c r="F27" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G27" s="1" t="n">
         <f aca="false">A17</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H27" s="1" t="n">
         <f aca="false">B17</f>
@@ -1578,116 +1584,116 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C28" s="1" t="str">
-        <v>François Lavoie</v>
+        <v>Absent Absent</v>
       </c>
       <c r="D28" s="5"/>
       <c r="F28" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G28" s="1" t="n">
         <f aca="false">A18</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H28" s="1" t="n">
         <f aca="false">B18</f>
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="I28" s="1" t="n">
         <f aca="false">D18</f>
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="C29" s="1" t="str">
-        <v>NA Les Méthos précieux</v>
-      </c>
-      <c r="D29" s="5" t="n">
-        <v>40</v>
-      </c>
+        <v>François Sergerie</v>
+      </c>
+      <c r="D29" s="5"/>
       <c r="F29" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G29" s="1" t="n">
         <f aca="false">A19</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H29" s="1" t="n">
         <f aca="false">B19</f>
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="I29" s="1" t="n">
         <f aca="false">D19</f>
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B30" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C30" s="1" t="e">
-        <v>#N/A</v>
+      <c r="A30" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <v>Arnaud Bouchard-Santerre</v>
       </c>
       <c r="D30" s="5"/>
       <c r="F30" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G30" s="1" t="n">
         <f aca="false">A20</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H30" s="1" t="n">
         <f aca="false">B20</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30" s="1" t="n">
         <f aca="false">D20</f>
-        <v>80</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B31" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C31" s="1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D31" s="5"/>
+      <c r="A31" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="C31" s="1" t="str">
+        <v>NA Les 12e meilleurs</v>
+      </c>
+      <c r="D31" s="5" t="n">
+        <v>50</v>
+      </c>
       <c r="F31" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G31" s="1" t="n">
         <f aca="false">A21</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H31" s="1" t="n">
         <f aca="false">B21</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I31" s="1" t="n">
         <f aca="false">D21</f>
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,70 +1709,70 @@
       <c r="D32" s="5"/>
       <c r="F32" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G32" s="1" t="n">
         <f aca="false">A22</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H32" s="1" t="n">
         <f aca="false">B22</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I32" s="1" t="n">
         <f aca="false">D22</f>
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="5"/>
       <c r="F33" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G33" s="1" t="n">
         <f aca="false">A23</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H33" s="1" t="n">
         <f aca="false">B23</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I33" s="1" t="n">
         <f aca="false">D23</f>
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F34" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G34" s="1" t="n">
         <f aca="false">A24</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H34" s="1" t="n">
         <f aca="false">B24</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I34" s="1" t="n">
         <f aca="false">D24</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G35" s="1" t="n">
         <f aca="false">A25</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H35" s="1" t="n">
         <f aca="false">B25</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I35" s="1" t="n">
         <f aca="false">D25</f>
@@ -1776,15 +1782,15 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F36" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G36" s="1" t="n">
         <f aca="false">A26</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">B26</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I36" s="1" t="n">
         <f aca="false">D26</f>
@@ -1794,15 +1800,15 @@
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F37" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G37" s="1" t="n">
         <f aca="false">A27</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">B27</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I37" s="1" t="n">
         <f aca="false">D27</f>
@@ -1812,15 +1818,15 @@
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F38" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G38" s="1" t="n">
         <f aca="false">A28</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H38" s="1" t="n">
         <f aca="false">B28</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I38" s="1" t="n">
         <f aca="false">D28</f>
@@ -1830,33 +1836,33 @@
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F39" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G39" s="1" t="n">
         <f aca="false">A29</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H39" s="1" t="n">
         <f aca="false">B29</f>
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="I39" s="1" t="n">
         <f aca="false">D29</f>
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F40" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
-      </c>
-      <c r="G40" s="1" t="e">
+        <v>5</v>
+      </c>
+      <c r="G40" s="1" t="n">
         <f aca="false">A30</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H40" s="1" t="e">
+        <v>6</v>
+      </c>
+      <c r="H40" s="1" t="n">
         <f aca="false">B30</f>
-        <v>#N/A</v>
+        <v>12</v>
       </c>
       <c r="I40" s="1" t="n">
         <f aca="false">D30</f>
@@ -1866,25 +1872,25 @@
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F41" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
-      </c>
-      <c r="G41" s="1" t="e">
+        <v>5</v>
+      </c>
+      <c r="G41" s="1" t="n">
         <f aca="false">A31</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H41" s="1" t="e">
+        <v>6</v>
+      </c>
+      <c r="H41" s="1" t="n">
         <f aca="false">B31</f>
-        <v>#N/A</v>
+        <v>99</v>
       </c>
       <c r="I41" s="1" t="n">
         <f aca="false">D31</f>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F42" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G42" s="1" t="e">
         <f aca="false">A32</f>
@@ -1902,7 +1908,7 @@
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F43" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G43" s="1" t="n">
         <f aca="false">A33</f>
@@ -1920,7 +1926,7 @@
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F44" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G44" s="1" t="n">
         <f aca="false">A34</f>
@@ -1938,7 +1944,7 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F45" s="1" t="n">
         <f aca="false">$B$2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G45" s="1" t="n">
         <f aca="false">A35</f>
@@ -2034,7 +2040,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -2052,7 +2058,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
@@ -2070,7 +2076,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
@@ -2088,7 +2094,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>19</v>
@@ -2106,7 +2112,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
@@ -2156,10 +2162,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="1" sqref="K4:K13 B43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="K4:K13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3166,13 +3172,13 @@
         <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>54</v>
@@ -3544,13 +3550,13 @@
         <v>99</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>54</v>
@@ -4000,13 +4006,13 @@
         <v>99</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>54</v>
@@ -4380,13 +4386,13 @@
         <v>99</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>54</v>
@@ -4874,13 +4880,13 @@
         <v>99</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>54</v>
@@ -5099,16 +5105,16 @@
         <v>7</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>46</v>
+        <v>144</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>47</v>
@@ -5125,11 +5131,11 @@
       </c>
       <c r="J73" s="1" t="n">
         <f aca="false">tblJoueurs!$B73</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K73" s="1" t="str">
         <f aca="false">tblJoueurs!$D73 &amp; " " &amp;tblJoueurs!$C73</f>
-        <v>Absent Absent</v>
+        <v>Yves Gilbert</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5137,16 +5143,16 @@
         <v>7</v>
       </c>
       <c r="B74" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>47</v>
@@ -5163,11 +5169,11 @@
       </c>
       <c r="J74" s="1" t="n">
         <f aca="false">tblJoueurs!$B74</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K74" s="1" t="str">
         <f aca="false">tblJoueurs!$D74 &amp; " " &amp;tblJoueurs!$C74</f>
-        <v>Catherine NA</v>
+        <v>Absent Absent</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5175,16 +5181,16 @@
         <v>7</v>
       </c>
       <c r="B75" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>144</v>
+        <v>41</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>144</v>
+        <v>41</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>47</v>
@@ -5201,11 +5207,11 @@
       </c>
       <c r="J75" s="1" t="n">
         <f aca="false">tblJoueurs!$B75</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K75" s="1" t="str">
         <f aca="false">tblJoueurs!$D75 &amp; " " &amp;tblJoueurs!$C75</f>
-        <v>Louis NA</v>
+        <v>Catherine NA</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5213,16 +5219,16 @@
         <v>7</v>
       </c>
       <c r="B76" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>47</v>
@@ -5239,11 +5245,11 @@
       </c>
       <c r="J76" s="1" t="n">
         <f aca="false">tblJoueurs!$B76</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K76" s="1" t="str">
         <f aca="false">tblJoueurs!$D76 &amp; " " &amp;tblJoueurs!$C76</f>
-        <v>Étienne Lemyre (Faciles)</v>
+        <v>Louis NA</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5251,16 +5257,16 @@
         <v>7</v>
       </c>
       <c r="B77" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>47</v>
@@ -5277,11 +5283,11 @@
       </c>
       <c r="J77" s="1" t="n">
         <f aca="false">tblJoueurs!$B77</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K77" s="1" t="str">
         <f aca="false">tblJoueurs!$D77 &amp; " " &amp;tblJoueurs!$C77</f>
-        <v>Élizabeth LeBlanc</v>
+        <v>Étienne Lemyre (Faciles)</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5289,19 +5295,19 @@
         <v>7</v>
       </c>
       <c r="B78" s="1" t="n">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>23</v>
+        <v>148</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>23</v>
+        <v>149</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G78" s="1" t="n">
         <v>1</v>
@@ -5315,25 +5321,49 @@
       </c>
       <c r="J78" s="1" t="n">
         <f aca="false">tblJoueurs!$B78</f>
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="K78" s="1" t="str">
         <f aca="false">tblJoueurs!$D78 &amp; " " &amp;tblJoueurs!$C78</f>
-        <v>NA Les Faciles à cuire</v>
+        <v>Élizabeth LeBlanc</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B79" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G79" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="I79" s="1" t="n">
         <f aca="false">tblJoueurs!$A79</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J79" s="1" t="n">
         <f aca="false">tblJoueurs!$B79</f>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="K79" s="1" t="str">
         <f aca="false">tblJoueurs!$D79 &amp; " " &amp;tblJoueurs!$C79</f>
-        <v> </v>
+        <v>NA Les Faciles à cuire</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5389,6 +5419,20 @@
       </c>
       <c r="K83" s="1" t="str">
         <f aca="false">tblJoueurs!$D83 &amp; " " &amp;tblJoueurs!$C83</f>
+        <v> </v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I84" s="1" t="n">
+        <f aca="false">tblJoueurs!$A84</f>
+        <v>0</v>
+      </c>
+      <c r="J84" s="1" t="n">
+        <f aca="false">tblJoueurs!$B84</f>
+        <v>0</v>
+      </c>
+      <c r="K84" s="1" t="str">
+        <f aca="false">tblJoueurs!$D84 &amp; " " &amp;tblJoueurs!$C84</f>
         <v> </v>
       </c>
     </row>
@@ -5514,13 +5558,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>47</v>
@@ -5647,10 +5691,10 @@
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>47</v>
@@ -5696,13 +5740,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>47</v>
@@ -5774,7 +5818,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>125</v>
@@ -6060,13 +6104,13 @@
         <v>99</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>54</v>
@@ -6242,13 +6286,13 @@
         <v>99</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>54</v>
@@ -6476,13 +6520,13 @@
         <v>99</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>54</v>
@@ -6710,13 +6754,13 @@
         <v>99</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>54</v>
@@ -6840,7 +6884,7 @@
         <v>6</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>125</v>
@@ -6892,13 +6936,13 @@
         <v>99</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>54</v>
@@ -7256,13 +7300,13 @@
         <v>12</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>47</v>

</xml_diff>